<commit_message>
push 5th version of the doc
</commit_message>
<xml_diff>
--- a/Documentation/PlanificationDétaillée.xlsx
+++ b/Documentation/PlanificationDétaillée.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Semaine 1" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -573,109 +573,76 @@
   </cellStyleXfs>
   <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -684,6 +651,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1005,15 +1005,15 @@
       <c r="A2" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="32" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1021,111 +1021,111 @@
       <c r="A3" s="8">
         <v>0.36458333333333331</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="21"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0.36805555555555558</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="36" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>0.39930555555555558</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>0.40972222222222227</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>0.44097222222222227</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>0.44444444444444442</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>0.47569444444444442</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>0.5625</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="21" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1133,73 +1133,73 @@
       <c r="A13" s="8">
         <v>0.59375</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="21"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>0.59722222222222221</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="21"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>0.62847222222222221</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="21"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>0.63888888888888895</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="23"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="24"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>0.67013888888888884</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="23"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>0.67361111111111116</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="23"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>0.70486111111111116</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="24"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1225,7 +1225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F19"/>
     </sheetView>
   </sheetViews>
@@ -1249,7 +1249,7 @@
         <v>44691</v>
       </c>
       <c r="D1" s="4">
-        <f t="shared" ref="D1:F1" si="0">C1+1</f>
+        <f t="shared" ref="D1:E1" si="0">C1+1</f>
         <v>44692</v>
       </c>
       <c r="E1" s="4">
@@ -1265,15 +1265,15 @@
       <c r="A2" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="32" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1281,109 +1281,109 @@
       <c r="A3" s="8">
         <v>0.36458333333333331</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="21"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0.36805555555555558</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="14" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>0.39930555555555558</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>0.40972222222222227</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>0.44097222222222227</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>0.44444444444444442</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>0.47569444444444442</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>0.5625</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="32" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1391,71 +1391,71 @@
       <c r="A13" s="8">
         <v>0.59375</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="21"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>0.59722222222222221</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="21"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>0.62847222222222221</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="21"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>0.63888888888888895</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="23"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="24"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>0.67013888888888884</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="23"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>0.67361111111111116</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="23"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>0.70486111111111116</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="24"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1518,15 +1518,15 @@
       <c r="A2" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="32" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1534,109 +1534,109 @@
       <c r="A3" s="8">
         <v>0.36458333333333331</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="21"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0.36805555555555558</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="14" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>0.39930555555555558</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>0.40972222222222227</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>0.44097222222222227</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>0.44444444444444442</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>0.47569444444444442</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>0.5625</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="32" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1644,71 +1644,71 @@
       <c r="A13" s="8">
         <v>0.59375</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="21"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>0.59722222222222221</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="21"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>0.62847222222222221</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="21"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>0.63888888888888895</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="23"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="24"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>0.67013888888888884</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="23"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>0.67361111111111116</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="23"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>0.70486111111111116</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="24"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1772,15 +1772,15 @@
       <c r="A2" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="42" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1788,109 +1788,109 @@
       <c r="A3" s="8">
         <v>0.36458333333333331</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0.36805555555555558</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="26" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="28"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>0.39930555555555558</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>0.40972222222222227</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>0.44097222222222227</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>0.44444444444444442</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>0.47569444444444442</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>0.5625</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="26" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="42" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1898,85 +1898,85 @@
       <c r="A13" s="8">
         <v>0.59375</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="34"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="45"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>0.59722222222222221</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="34"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="45"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>0.62847222222222221</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="34"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="45"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>0.63888888888888895</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="34"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="45"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>0.67013888888888884</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="34"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="45"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>0.67361111111111116</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="34"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="45"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>0.70486111111111116</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="35"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="C12:C19"/>
-    <mergeCell ref="E12:E19"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="F16:F19"/>
     <mergeCell ref="B2:B11"/>
     <mergeCell ref="C2:C11"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F9"/>
     <mergeCell ref="E4:E9"/>
     <mergeCell ref="E10:F11"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="E12:E19"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="F16:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1986,7 +1986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F19"/>
     </sheetView>
   </sheetViews>
@@ -2026,15 +2026,15 @@
       <c r="A2" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="42" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2042,109 +2042,109 @@
       <c r="A3" s="8">
         <v>0.36458333333333331</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0.36805555555555558</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="26" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="28"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>0.39930555555555558</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>0.40972222222222227</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>0.44097222222222227</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>0.44444444444444442</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>0.47569444444444442</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>0.5625</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="26" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="42" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2152,85 +2152,85 @@
       <c r="A13" s="8">
         <v>0.59375</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="34"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="45"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>0.59722222222222221</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="34"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="45"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>0.62847222222222221</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="34"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="45"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>0.63888888888888895</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="34"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="45"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>0.67013888888888884</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="34"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="45"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>0.67361111111111116</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="34"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="45"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>0.70486111111111116</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="35"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="C12:C19"/>
-    <mergeCell ref="E12:E19"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="F16:F19"/>
     <mergeCell ref="B2:B11"/>
     <mergeCell ref="C2:C11"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F9"/>
     <mergeCell ref="E4:E9"/>
     <mergeCell ref="E10:F11"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="C12:C19"/>
+    <mergeCell ref="E12:E19"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="F16:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>